<commit_message>
Fixed get monthly reports & between dates reports, and showing them as charts
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saman\Desktop\BI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saman\Desktop\projects\BI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>groupID</t>
   </si>
@@ -72,6 +72,27 @@
   </si>
   <si>
     <t>امنیت شبکه  10006در دنیای موازی چیست؟</t>
+  </si>
+  <si>
+    <t>برنامه نویسی</t>
+  </si>
+  <si>
+    <t>طراحی سایت</t>
+  </si>
+  <si>
+    <t>چند درصد وب سایت های دنیا توسط وردپرس توسعه داده شدند؟</t>
+  </si>
+  <si>
+    <t>ورد پرس</t>
+  </si>
+  <si>
+    <t>دوآپس</t>
+  </si>
+  <si>
+    <t>CI/CD</t>
+  </si>
+  <si>
+    <t>چند درصد وب سایت های دنیا توسط وردپرس توسعه داده شدند؟ 1</t>
   </si>
 </sst>
 </file>
@@ -389,17 +410,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
     <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -515,6 +536,34 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some texts in req.flash() and some bugs in whole project
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saman\Desktop\projects\BI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\BI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>groupID</t>
   </si>
@@ -38,68 +38,23 @@
     <t>description</t>
   </si>
   <si>
-    <t>زیرساخت</t>
-  </si>
-  <si>
-    <t>امنیت شبکه</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  3در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  4در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  5در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>معماری</t>
-  </si>
-  <si>
-    <t>نرم افزار Auto Cad</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  10002در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  10003در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  10004در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  10005در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>امنیت شبکه  10006در دنیای موازی چیست؟</t>
-  </si>
-  <si>
-    <t>برنامه نویسی</t>
-  </si>
-  <si>
-    <t>طراحی سایت</t>
-  </si>
-  <si>
-    <t>چند درصد وب سایت های دنیا توسط وردپرس توسعه داده شدند؟</t>
-  </si>
-  <si>
-    <t>ورد پرس</t>
-  </si>
-  <si>
-    <t>دوآپس</t>
-  </si>
-  <si>
-    <t>CI/CD</t>
-  </si>
-  <si>
-    <t>چند درصد وب سایت های دنیا توسط وردپرس توسعه داده شدند؟ 1</t>
+    <t>نام گروه</t>
+  </si>
+  <si>
+    <t>نام زیرگروه</t>
+  </si>
+  <si>
+    <t>متن سوال</t>
+  </si>
+  <si>
+    <t>متن توضیحات سوال</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,16 +62,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Vazir"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -124,12 +91,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,161 +399,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Favicon, added a useful feature when uploading excel files (xlsx)
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>groupID</t>
   </si>
@@ -38,16 +38,217 @@
     <t>description</t>
   </si>
   <si>
-    <t>نام گروه</t>
-  </si>
-  <si>
-    <t>نام زیرگروه</t>
-  </si>
-  <si>
-    <t>متن سوال</t>
-  </si>
-  <si>
-    <t>متن توضیحات سوال</t>
+    <t>ریاضیات</t>
+  </si>
+  <si>
+    <t>جبر</t>
+  </si>
+  <si>
+    <t>حاصل جمع 5 و 7 چند است؟</t>
+  </si>
+  <si>
+    <t>این سؤال مربوط به عملیات ساده جمع در جبر است.</t>
+  </si>
+  <si>
+    <t>هندسه</t>
+  </si>
+  <si>
+    <t>مساحت یک مربع با ضلع 4 سانتی‌متر چقدر است؟</t>
+  </si>
+  <si>
+    <t>این سؤال درباره محاسبه مساحت مربع است.</t>
+  </si>
+  <si>
+    <t>علوم تجربی</t>
+  </si>
+  <si>
+    <t>زیست‌شناسی</t>
+  </si>
+  <si>
+    <t>کدام عضو بدن وظیفه پمپاژ خون را بر عهده دارد؟</t>
+  </si>
+  <si>
+    <t>این سؤال مربوط به سیستم گردش خون بدن است.</t>
+  </si>
+  <si>
+    <t>شیمی</t>
+  </si>
+  <si>
+    <t>فرمول شیمیایی آب چیست؟</t>
+  </si>
+  <si>
+    <t>این سؤال برای سنجش دانش شیمی پایه است.</t>
+  </si>
+  <si>
+    <t>تاریخ</t>
+  </si>
+  <si>
+    <t>تاریخ ایران</t>
+  </si>
+  <si>
+    <t>سلسله صفویه در چه قرنی تأسیس شد؟</t>
+  </si>
+  <si>
+    <t>این سؤال به تاریخ ایران مرتبط است.</t>
+  </si>
+  <si>
+    <t>تاریخ جهان</t>
+  </si>
+  <si>
+    <t>جنگ جهانی دوم در چه سالی آغاز شد؟</t>
+  </si>
+  <si>
+    <t>این سؤال به تاریخ معاصر جهان اشاره دارد.</t>
+  </si>
+  <si>
+    <t>کامپیوتر</t>
+  </si>
+  <si>
+    <t>سخت‌افزار</t>
+  </si>
+  <si>
+    <t>CPU مخفف چیست؟</t>
+  </si>
+  <si>
+    <t>این سؤال درباره شناخت اجزای سخت‌افزاری است.</t>
+  </si>
+  <si>
+    <t>حافظه RAM چه وظیفه‌ای دارد؟</t>
+  </si>
+  <si>
+    <t>درباره مفهوم و کارکرد RAM توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>SSD چه تفاوتی با HDD دارد؟</t>
+  </si>
+  <si>
+    <t>مربوط به فناوری‌های ذخیره‌سازی است.</t>
+  </si>
+  <si>
+    <t>نرم‌افزار</t>
+  </si>
+  <si>
+    <t>سیستم‌عامل چیست؟</t>
+  </si>
+  <si>
+    <t>این سؤال درباره تعریف سیستم‌عامل است.</t>
+  </si>
+  <si>
+    <t>مثال‌هایی از نرم‌افزارهای متن‌باز کدام‌اند؟</t>
+  </si>
+  <si>
+    <t>درباره نرم‌افزارهای Open Source است.</t>
+  </si>
+  <si>
+    <t>شبکه</t>
+  </si>
+  <si>
+    <t>پروتکل TCP/IP چیست؟</t>
+  </si>
+  <si>
+    <t>این سؤال به شبکه‌های کامپیوتری مربوط است.</t>
+  </si>
+  <si>
+    <t>تفاوت بین LAN و WAN چیست؟</t>
+  </si>
+  <si>
+    <t>درباره انواع شبکه‌ها توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>سوئیچ در شبکه چه کاربردی دارد؟</t>
+  </si>
+  <si>
+    <t>این سؤال به مفاهیم شبکه اشاره دارد.</t>
+  </si>
+  <si>
+    <t>برنامه‌نویسی</t>
+  </si>
+  <si>
+    <t>زبان برنامه‌نویسی Python در چه حوزه‌هایی کاربرد دارد؟</t>
+  </si>
+  <si>
+    <t>درباره کاربردهای پایتون توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>حلقه for چه کاربردی در برنامه‌نویسی دارد؟</t>
+  </si>
+  <si>
+    <t>این سؤال به مفاهیم پایه‌ای برنامه‌نویسی مربوط است.</t>
+  </si>
+  <si>
+    <t>پایگاه‌داده</t>
+  </si>
+  <si>
+    <t>تفاوت بین SQL و NoSQL چیست؟</t>
+  </si>
+  <si>
+    <t>به مفاهیم پایگاه داده‌های رابطه‌ای و غیررابطه‌ای اشاره دارد.</t>
+  </si>
+  <si>
+    <t>یک مثال از دستور SELECT در SQL چیست؟</t>
+  </si>
+  <si>
+    <t>درباره نحوه کار با پایگاه داده توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>هوش مصنوعی</t>
+  </si>
+  <si>
+    <t>یادگیری ماشین چیست؟</t>
+  </si>
+  <si>
+    <t>این سؤال درباره مفاهیم ابتدایی هوش مصنوعی است.</t>
+  </si>
+  <si>
+    <t>تفاوت بین یادگیری نظارت‌شده و بدون نظارت چیست؟</t>
+  </si>
+  <si>
+    <t>درباره روش‌های یادگیری ماشین توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>اینترنت</t>
+  </si>
+  <si>
+    <t>مرورگر وب چه وظیفه‌ای دارد؟</t>
+  </si>
+  <si>
+    <t>این سؤال به کارکرد مرورگرها اشاره دارد.</t>
+  </si>
+  <si>
+    <t>تفاوت HTTP و HTTPS چیست؟</t>
+  </si>
+  <si>
+    <t>درباره پروتکل‌های اینترنت توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>امنیت سایبری</t>
+  </si>
+  <si>
+    <t>فایروال چیست و چگونه کار می‌کند؟</t>
+  </si>
+  <si>
+    <t>این سؤال به اصول امنیت سایبری مربوط است.</t>
+  </si>
+  <si>
+    <t>چرا باید از رمزهای عبور قوی استفاده کنیم؟</t>
+  </si>
+  <si>
+    <t>درباره اهمیت رمزنگاری و امنیت توضیح می‌دهد.</t>
+  </si>
+  <si>
+    <t>گرافیک کامپیوتری</t>
+  </si>
+  <si>
+    <t>تفاوت بین فرمت‌های PNG و JPEG چیست؟</t>
+  </si>
+  <si>
+    <t>به اصول گرافیک کامپیوتری مربوط است.</t>
+  </si>
+  <si>
+    <t>GPU چه نقشی در کامپیوتر دارد؟</t>
+  </si>
+  <si>
+    <t>این سؤال درباره پردازنده گرافیکی است.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -118,6 +319,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A8" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.5"/>
@@ -430,17 +634,373 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.5">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.5">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.5">
+      <c r="A16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="120" x14ac:dyDescent="0.5">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.5">
+      <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.5">
+      <c r="A23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.5">
+      <c r="A26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.5">
+      <c r="A28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>